<commit_message>
Created DB connection REST API v1
</commit_message>
<xml_diff>
--- a/Documentation/DatabasePreparation/DatabaseArchitecture.xlsx
+++ b/Documentation/DatabasePreparation/DatabaseArchitecture.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" tabRatio="887" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" tabRatio="887" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Library" sheetId="5" r:id="rId9"/>
     <sheet name="LabHours" sheetId="11" r:id="rId10"/>
     <sheet name="LibraryHours" sheetId="12" r:id="rId11"/>
+    <sheet name="LibraryRooms" sheetId="13" r:id="rId12"/>
+    <sheet name="RoomReservation" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -463,6 +465,36 @@
   </si>
   <si>
     <t>2016-03-18T18:00:00Z</t>
+  </si>
+  <si>
+    <t>RoomNumber</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Projector</t>
+  </si>
+  <si>
+    <t>402B</t>
+  </si>
+  <si>
+    <t>Room_ID</t>
+  </si>
+  <si>
+    <t>2016-03-12T12:00:00Z</t>
+  </si>
+  <si>
+    <t>2016-03-12T10:00:00Z</t>
+  </si>
+  <si>
+    <t>2016-03-16T09:00:00Z</t>
+  </si>
+  <si>
+    <t>2016-03-18T11:00:00Z</t>
+  </si>
+  <si>
+    <t>2016-03-12T13:00:00Z</t>
   </si>
 </sst>
 </file>
@@ -507,10 +539,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1056,7 +1091,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,11 +1243,220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>303</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>209</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>